<commit_message>
Refactor code to save data to JSON file
</commit_message>
<xml_diff>
--- a/temp_output.xlsx
+++ b/temp_output.xlsx
@@ -471,19 +471,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vo Quoc Khanh</t>
+          <t>a</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-04-01 00:00:00</t>
+          <t>2024-11-11 00:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add search functionality and update UI
</commit_message>
<xml_diff>
--- a/temp_output.xlsx
+++ b/temp_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,14 +476,374 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t xml:space="preserve"> Tạp chí Văn hóa – Văn nghệ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-11-11 00:00:00</t>
+          <t>2024-01-14 16:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thế giới chuyển động</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024-01-14 16:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> An toàn giao thông</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024-01-14 16:29:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Phim Khi nắng thu về</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024-01-14 16:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> An ninh Hậu Giang</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024-01-14 18:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> VFC cánh đồng hội nhập</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024-01-14 18:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tin tức Mekong</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://60acee235f4d5.streamlock.net:443/VODHGTV/definst/VIDEO/mp4:ttmk-140124.mp4/playlist.m3u8</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024-01-14 18:29:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Tiếp chuyển Thời sự VTV</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024-01-14 19:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thời sự Hậu Giang – Thời tiết nông vụ</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://60acee235f4d5.streamlock.net:443/VODHGTV/definst/VIDEO/mp4:tshg-140124.mp4/playlist.m3u8</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2024-01-14 19:40:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Hậu Giang trên đường phát triển</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2024-01-14 20:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Phim tài liệu 20 năm thành lập tỉnh Hậu Giang (T10)</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2024-01-14 20:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Phim Huynh đệ tương tàn (T18,19)</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2024-01-14 20:50:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thế giới chuyển động</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2024-01-14 22:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> VFC cánh đồng hội nhập</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2024-01-14 22:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Chuyện tình tôi kể</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2024-01-14 22:45:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Phim tài liệU</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2024-01-14 23:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Trích đoạn sân khấu</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2024-01-14 23:30:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update schedule TV UI and data
</commit_message>
<xml_diff>
--- a/temp_output.xlsx
+++ b/temp_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,374 +476,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Tạp chí Văn hóa – Văn nghệ</t>
+          <t>alo</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-01-14 16:00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Thế giới chuyển động</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-01-14 16:15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> An toàn giao thông</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2024-01-14 16:29:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Phim Khi nắng thu về</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2024-01-14 16:30:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> An ninh Hậu Giang</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2024-01-14 18:00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> VFC cánh đồng hội nhập</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2024-01-14 18:15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Tin tức Mekong</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>https://60acee235f4d5.streamlock.net:443/VODHGTV/definst/VIDEO/mp4:ttmk-140124.mp4/playlist.m3u8</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2024-01-14 18:29:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Tiếp chuyển Thời sự VTV</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2024-01-14 19:00:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Thời sự Hậu Giang – Thời tiết nông vụ</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>https://60acee235f4d5.streamlock.net:443/VODHGTV/definst/VIDEO/mp4:tshg-140124.mp4/playlist.m3u8</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2024-01-14 19:40:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Hậu Giang trên đường phát triển</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2024-01-14 20:15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Phim tài liệu 20 năm thành lập tỉnh Hậu Giang (T10)</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2024-01-14 20:30:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Phim Huynh đệ tương tàn (T18,19)</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2024-01-14 20:50:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Thế giới chuyển động</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2024-01-14 22:15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> VFC cánh đồng hội nhập</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2024-01-14 22:30:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Chuyện tình tôi kể</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2024-01-14 22:45:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Phim tài liệU</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2024-01-14 23:15:00</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Trích đoạn sân khấu</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2024-01-14 23:30:00</t>
+          <t>2024-01-12 00:00:00</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new files and update requirements.txt
</commit_message>
<xml_diff>
--- a/temp_output.xlsx
+++ b/temp_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,19 +471,757 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>alo</t>
+          <t>Chương trình Tam nông</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://60acee235f4d5.streamlock.net:443/VODHGTV/definst/AUDIO/mp3:tamnong-140124.mp3/playlist.m3u8</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-01-12 00:00:00</t>
+          <t>2024-01-14 05:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Trực tiếp Thời sự sáng</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2024-01-14 05:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tiếp âm thời sự Đài Tiếng nói VN</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2024-01-14 06:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Điều con muốn – Đừng ước mơ thay con</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024-01-14 06:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Tập 2 phim ngắn Chuyện quê mình</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024-01-14 06:45:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Nhạc quê hương – Tình vợ chồng quê</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2024-01-14 07:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Tạp chí văn hóa văn nghệ</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2024-01-14 07:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sân khấu</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2024-01-14 07:45:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alo bác sĩ ơi -  Thoái hoa khớp</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2024-01-14 09:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Pháp luật với công dân</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2024-01-14 10:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Hành trình cung bậc phương Nam</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2024-01-14 10:05:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Chuyên đề Hành trình OCOP</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2024-01-14 10:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Noi theo gương sáng Bác Hồ</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2024-01-14 10:45:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Chương trình ca cổ - Một khúc ca</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2024-01-14 11:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Trực tiếp Thời sự trưa</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2024-01-14 11:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Tiếp âm TS Đài TNVN</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2024-01-14 12:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Nhạc quê hương – Tình vợ chồng quê</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2024-01-14 13:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Tạp chí văn hóa văn nghệ</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2024-01-14 13:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Sân khấu</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2024-01-14 13:45:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bản tin phòng chống thiên tai dịch bệnh,</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2024-01-14 15:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Bản tin Cẩm nang mua sắm</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2024-01-14 15:45:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Pháp luật với công dân</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2024-01-14 16:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Điều con muốn – Đừng ước mơ thay con</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2024-01-14 16:05:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Tập 2 phim ngắn Chuyện quê mình</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2024-01-14 16:15:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Chương trình Tam nông</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>https://60acee235f4d5.streamlock.net:443/VODHGTV/definst/AUDIO/mp3:tamnong-140124.mp3/playlist.m3u8</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2024-01-14 16:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Chương trình ca cổ - Một khúc ca</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2024-01-14 17:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Thời sự chiều</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2024-01-14 17:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Tiếp âm Đài TNVN</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2024-01-14 18:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Alo bác sĩ ơi -  Thoái hoa khớp</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2024-01-14 19:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Sắc màu văn học</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>https://60acee235f4d5.streamlock.net:443/VODHGTV/definst/AUDIO/mp3:smvh-20h-140124.mp3/playlist.m3u8</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2024-01-14 20:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Tài tử miệt vườn.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2024-01-14 20:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Tiếp âm thời sự đài tiếng nói Việt Nam</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2024-01-14 21:30:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Chuyện tình tôi kể.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2024-01-14 22:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Sắc màu văn học, truyện Mật mã Tây Tạng của tác giả Hà Mã</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2024-01-14 22:30:00</t>
         </is>
       </c>
     </row>

</xml_diff>